<commit_message>
🤖 Publica dados no site (08/11/2025 10:09)
</commit_message>
<xml_diff>
--- a/site/downloads/HCPA.xlsx
+++ b/site/downloads/HCPA.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HCPA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HCPA — Acesso Direto" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HCPA — Pré-Requisito" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1008,4 +1009,1343 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PROGRAMA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>VAGAS DISPONÍVEIS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CANDIDATOS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CONCORRÊNCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cardiologia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>11,17</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cirurgia de Cabeça e Pescoço</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cirurgia do Aparelho Digestivo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cirurgia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cirurgia Plástica</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cirurgia Torácica</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cirurgia Vascular</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Coloproctologia</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Endocrinologia e Metabologia</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>17,67</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Gastroenterologia</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>10,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Geriatria</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Hematologia e Hemoterapia</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Mastologia</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nefrologia</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4,2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Oncologia Clínica</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Oncologia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Pneumologia</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>7,4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Reumatologia</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Urologia</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>10,67</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Administração em Saúde</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Angiorradiologia e Cirurgia Endovascular</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Cirurgia Craniomaxilofacial</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Dor</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Ecocardiografia</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>6,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Eletrofisiologia Clínica Invasiva</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Emergência Pediátrica</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Endocrinologia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Endoscopia Digestiva</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>3,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Endoscopia Ginecológica</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Endoscopia Respiratória</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Endoscopia Respiratória</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ergometria</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Gastroenterologia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Hematologia e Hemoterapia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Hemodinâmica e Cardiologia Intervencionista</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Hepatologia</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Infectologia Hospitalar</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Medicina Fetal</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Medicina Intensiva Pediátrica</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Medicina Paliativa</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>1,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Neonatologia</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>1,8</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Neurofisiologia Clínica</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Neurologia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>14,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Nutrologia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Pneumologia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>1,67</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Psicoterapia</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Psiquiatria da Infância e Adolescência</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Psiquiatria Forense</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Reprodução Assistida</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Reumatologia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Transplante de Fígado</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Transplante de Medula Óssea</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Clínica Médica (Ano Adicional)</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0,67</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Ginecologia e Obstetrícia (Ano Adicional)</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Psiquiatria (Ano Adicional)</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Transplante de Coração (Ano Adicional)</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Transplante de Córnea (Ano Adicional)</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Transplante Renal (Ano Adicional)</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Transplante Renal (Ano Adicional)</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>